<commit_message>
updated tests to handle new template format
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/FashionValley_one_conc.xlsx
+++ b/tests/testthat/test_data/FashionValley_one_conc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/BMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/BMP/FWCCalculator/tests/testthat/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{4BB56CD4-6890-470F-9E51-CD928D1F5467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2210037-1874-45FC-80CD-FB964E259BAB}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{4BB56CD4-6890-470F-9E51-CD928D1F5467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2C4BD07-0080-42B1-858B-8498F9644E4F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hydrograph" sheetId="1" r:id="rId1"/>
-    <sheet name="Pollutograph" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="3" r:id="rId1"/>
+    <sheet name="Hydrograph" sheetId="1" r:id="rId2"/>
+    <sheet name="Pollutograph" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,6 +117,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,10 +385,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2016F734-9287-4F62-B706-10B8E06405D2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B646"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6208,7 +6225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6F71FE-E1E7-4376-9B6B-E3EA018A2BD1}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -6427,6 +6444,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6686,15 +6712,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6709,6 +6726,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{851FA841-BED3-4AA9-8CA6-6B5F6DAC2D17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B58E0D-20BE-4A84-9419-20FAFBF18F8D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6728,14 +6753,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{851FA841-BED3-4AA9-8CA6-6B5F6DAC2D17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D782A14-F801-4D81-AC35-0B683C77D4CA}">
   <ds:schemaRefs>

</xml_diff>